<commit_message>
Cab booking select time problem fixed
</commit_message>
<xml_diff>
--- a/MakeMyTrip/ExcelData/makeMyTrip.xlsx
+++ b/MakeMyTrip/ExcelData/makeMyTrip.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitish verma\git\MakeMyTripSeleniumTesting\MakeMyTrip\ExcelData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC790142-1922-4703-92D7-BC25FDEB775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="13728" windowHeight="5580" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
@@ -12,9 +18,8 @@
     <sheet name="CAB" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L17"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -60,9 +65,6 @@
     <t>"26/07/2021"</t>
   </si>
   <si>
-    <t>"18/07/2021"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Senders Number </t>
   </si>
   <si>
@@ -94,16 +96,19 @@
   </si>
   <si>
     <t>mithai lelo</t>
+  </si>
+  <si>
+    <t>"28/07/2021"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]hh:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,27 +425,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -451,7 +456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -468,93 +473,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>19</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
       <c r="E2">
         <v>9044096545</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -576,10 +581,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3">
-        <v>0.77083333333333337</v>
+        <v>0.27083333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed with log4j,comments and grouping of 18 testcases into smoke and regression using suite
</commit_message>
<xml_diff>
--- a/MakeMyTrip/ExcelData/makeMyTrip.xlsx
+++ b/MakeMyTrip/ExcelData/makeMyTrip.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{323B3379-C76E-4E79-B9DF-0FD2FC27E3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="13728" windowHeight="5580" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13755" windowHeight="8985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
     <sheet name="GIFT CARD" sheetId="2" r:id="rId2"/>
     <sheet name="CAB" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1:L17"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -60,9 +61,6 @@
     <t>"26/07/2021"</t>
   </si>
   <si>
-    <t>"18/07/2021"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Senders Number </t>
   </si>
   <si>
@@ -94,16 +92,19 @@
   </si>
   <si>
     <t>mithai lelo</t>
+  </si>
+  <si>
+    <t>"28/07/2021"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]hh:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,27 +421,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -451,7 +452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -468,93 +469,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>19</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
       <c r="E2">
         <v>9044096545</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -576,7 +577,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3">
         <v>0.77083333333333337</v>

</xml_diff>